<commit_message>
Added structure and product ID for A14-4
</commit_message>
<xml_diff>
--- a/product_IDs_19_5_7_21.xlsx
+++ b/product_IDs_19_5_7_21.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Compound</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Z22148724</t>
+  </si>
+  <si>
+    <t>A14-4</t>
+  </si>
+  <si>
+    <t>Z45900028</t>
   </si>
 </sst>
 </file>
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,6 +506,14 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>